<commit_message>
Update source code into 1.01 version
* Reflect changes in the schema such as change Datasets into
ResourceTypes
* fix bugs in data loading
* fix bugs in the Installer (many windows didn't respond in the 1.0
version)
</commit_message>
<xml_diff>
--- a/WorkbookTemplates/Compare_scenarios_result/CompareScenario_empty.xlsx
+++ b/WorkbookTemplates/Compare_scenarios_result/CompareScenario_empty.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adel\Documents\GitHub\WamdamProject\WaMDaM_UseCases\UseCases_files\0WorkbookTemplates\Compare_scenarios_result\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adel\Documents\GitHub\WamdamProject\WaMDaM_Wizard\WorkbookTemplates\Compare_scenarios_result\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="ChangeInTopology" sheetId="1" r:id="rId1"/>
     <sheet name="ChangeInMetadata_Topology" sheetId="2" r:id="rId2"/>
     <sheet name="ChangeInMetadata_Attributes" sheetId="3" r:id="rId3"/>
-    <sheet name="ChangeInDataValues" sheetId="4" r:id="rId4"/>
+    <sheet name="ChangeInValues" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
@@ -687,7 +687,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1315,7 +1315,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>